<commit_message>
SSDM-55: fixed xls export types data.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type-compatible-with-import.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type-compatible-with-import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t xml:space="preserve">DATASET_TYPE</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dynamic script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multivalued</t>
   </si>
   <si>
     <t xml:space="preserve">$NAME</t>
@@ -119,10 +122,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -156,6 +160,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -201,7 +213,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -212,6 +224,14 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -231,13 +251,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4:L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -269,7 +289,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -303,93 +323,105 @@
       <c r="K4" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
+      <c r="L7" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>